<commit_message>
add x64 config file
</commit_message>
<xml_diff>
--- a/code/codeacad/docs/plans.xlsx
+++ b/code/codeacad/docs/plans.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="plans" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="bugs" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,9 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Acad auto run app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>custom menu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>custom toolbar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>custom others</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -376,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -396,6 +408,24 @@
         <v>42422</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42423</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -407,7 +437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>

</xml_diff>